<commit_message>
added more intermediate files to steepest descent
</commit_message>
<xml_diff>
--- a/02-lab/output/excel/steepest_descent_method_0_0.xlsx
+++ b/02-lab/output/excel/steepest_descent_method_0_0.xlsx
@@ -53,7 +53,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -61,6 +61,7 @@
   <cols>
     <col min="1" max="1" width="2.140625" customWidth="true"/>
     <col min="2" max="2" width="2.140625" customWidth="true"/>
+    <col min="3" max="3" width="2.85546875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -70,6 +71,9 @@
       <c r="B1" s="0">
         <v>0</v>
       </c>
+      <c r="C1" s="0">
+        <v>-1</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
@@ -78,6 +82,9 @@
       <c r="B2" s="0">
         <v>0</v>
       </c>
+      <c r="C2" s="0">
+        <v>3.8579502713798809e-05</v>
+      </c>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>